<commit_message>
error in logging in to login page
</commit_message>
<xml_diff>
--- a/test/testdata/testing_data.xlsx
+++ b/test/testdata/testing_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\repository\test\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nares\git\new-project\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36F2DC0-4E79-437E-9009-258EDB551358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F64B80-A4F5-4FFE-9D70-B5C850E83FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D0AD5B91-B4B7-4940-AED4-2C500B6CC9A1}"/>
+    <workbookView xWindow="1776" yWindow="1776" windowWidth="13320" windowHeight="9432" xr2:uid="{D0AD5B91-B4B7-4940-AED4-2C500B6CC9A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,25 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
-  <si>
-    <t>mobile number</t>
-  </si>
   <si>
     <t>result</t>
   </si>
@@ -47,6 +34,9 @@
   </si>
   <si>
     <t>fail</t>
+  </si>
+  <si>
+    <t>mobile_number</t>
   </si>
 </sst>
 </file>
@@ -402,52 +392,52 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>7032753299</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1231231233</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>12312312312333</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in external report generation
</commit_message>
<xml_diff>
--- a/test/testdata/testing_data.xlsx
+++ b/test/testdata/testing_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nares\git\new-project\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EF59E2-051B-4333-8978-2BAA02B6B98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C467047-0EA2-499C-94F1-9792A6D7B090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1776" yWindow="1776" windowWidth="13320" windowHeight="9432" xr2:uid="{D0AD5B91-B4B7-4940-AED4-2C500B6CC9A1}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,13 +31,13 @@
     <t>result</t>
   </si>
   <si>
-    <t>fail</t>
-  </si>
-  <si>
     <t>mobile_number</t>
   </si>
   <si>
     <t>pass</t>
+  </si>
+  <si>
+    <t>fail</t>
   </si>
 </sst>
 </file>
@@ -392,7 +393,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -402,7 +403,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -413,15 +414,15 @@
         <v>7032753299</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>1231231233</v>
+        <v>7897798797989</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -429,15 +430,15 @@
         <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>12312312312333</v>
+        <v>1234567890</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
running testcases using pom.xml file for the maven configuration
</commit_message>
<xml_diff>
--- a/test/testdata/testing_data.xlsx
+++ b/test/testdata/testing_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nares\git\new-project\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C467047-0EA2-499C-94F1-9792A6D7B090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02813662-190B-4886-B620-B1B15BEC6E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1776" yWindow="1776" windowWidth="13320" windowHeight="9432" xr2:uid="{D0AD5B91-B4B7-4940-AED4-2C500B6CC9A1}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -393,7 +392,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,7 +434,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>1234567890</v>
+        <v>33330000</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>

</xml_diff>